<commit_message>
Se integran las vistas de los niveles inferiores
</commit_message>
<xml_diff>
--- a/public/excel/Formato-BBDD-Gobiernos.xlsx
+++ b/public/excel/Formato-BBDD-Gobiernos.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19360" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Institución Educativa" sheetId="1" r:id="rId1"/>
-    <sheet name="Sedes" sheetId="2" r:id="rId2"/>
-    <sheet name="Docentes" sheetId="3" r:id="rId3"/>
+    <sheet name="Subdivisiones" sheetId="4" r:id="rId1"/>
+    <sheet name="Institución Educativa" sheetId="1" r:id="rId2"/>
+    <sheet name="Sedes" sheetId="2" r:id="rId3"/>
+    <sheet name="Docentes" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>País</t>
   </si>
@@ -143,13 +144,28 @@
   </si>
   <si>
     <t>Vereda</t>
+  </si>
+  <si>
+    <t>Tipo de primera división</t>
+  </si>
+  <si>
+    <t>Tipo de segunda división</t>
+  </si>
+  <si>
+    <t>Tipo de tercera división</t>
+  </si>
+  <si>
+    <t>Valle del Cauca</t>
+  </si>
+  <si>
+    <t>Muicipio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,6 +196,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -213,6 +237,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -493,6 +523,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -548,125 +620,135 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="7" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="34.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>1234567890</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>987654321</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -677,8 +759,9 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -689,8 +772,9 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -701,8 +785,9 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -713,8 +798,9 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -725,8 +811,9 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -737,8 +824,9 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -749,8 +837,9 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -761,8 +850,9 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -773,8 +863,9 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -785,8 +876,9 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -797,8 +889,9 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -809,19 +902,20 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="I2" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="I3" r:id="rId4"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId2"/>
+    <hyperlink ref="I3" r:id="rId3"/>
+    <hyperlink ref="J3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>

</xml_diff>